<commit_message>
Creating and Reading Excel using Apache POI
</commit_message>
<xml_diff>
--- a/src/test/java/utilities/Excelbook1.xlsx
+++ b/src/test/java/utilities/Excelbook1.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="Employee Data" r:id="rId3" sheetId="1"/>
+    <sheet name="Department Data" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>EmployeeNum</t>
   </si>
@@ -51,6 +52,60 @@
   </si>
   <si>
     <t>Emp105</t>
+  </si>
+  <si>
+    <t>DeptNum</t>
+  </si>
+  <si>
+    <t>DeptName</t>
+  </si>
+  <si>
+    <t>DeptLocation</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Dept10</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Dept20</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Dept30</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Dept40</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Dept50</t>
+  </si>
+  <si>
+    <t>Russia</t>
   </si>
 </sst>
 </file>
@@ -170,4 +225,83 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>